<commit_message>
Algoritmo de números amigos y toma de tiempos de ejecución con su gráfica
</commit_message>
<xml_diff>
--- a/numeros_amigos/Algoritmo de números amigos.xlsx
+++ b/numeros_amigos/Algoritmo de números amigos.xlsx
@@ -253,9 +253,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,6 +276,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,6 +294,970 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Gráfica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> de tallas vs promedio(segundos)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Hoja 1'!$B$4:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>220-284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1184-1210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2620-2924</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5020-5564</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6232-6368</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10744-10856</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12285-14595</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17296-18416</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63020-76084</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66928-66992</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.0959999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2079999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0025999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0446E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.0580000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>9.5340000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>9.8759999999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.637999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>8.4739999999999989E-3</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>8.7219999999999989E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E76-44B2-B2EB-BF3340810420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="196114480"/>
+        <c:axId val="196125296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="196114480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="196125296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="196125296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="196114480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,37 +1464,37 @@
   <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="10" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="12"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,298 +1519,298 @@
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1.0630000000000001E-2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>8.6E-3</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <f t="shared" ref="H4:H13" si="0">AVERAGE(C4:G4)</f>
         <v>9.0959999999999999E-3</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1.0710000000000001E-2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1.031E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>8.1899999999999994E-3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>8.43E-3</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <f t="shared" si="0"/>
         <v>9.2079999999999992E-3</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1.068E-2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1.2319999999999999E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>8.4899999999999993E-3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>8.4399999999999996E-3</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>1.0025999999999998E-2</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1.022E-2</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1.1129999999999999E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1.0460000000000001E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1.0410000000000001E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>1.001E-2</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <f t="shared" si="0"/>
         <v>1.0446E-2</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>9.9500000000000005E-3</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>8.4899999999999993E-3</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>8.8500000000000002E-3</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>8.8199999999999997E-3</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>9.1800000000000007E-3</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>9.0580000000000001E-3</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1.0059999999999999E-2</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>8.7799999999999996E-3</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>8.6E-3</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>9.2300000000000004E-3</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>9.5340000000000008E-3</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1.1050000000000001E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>9.6900000000000007E-3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>1.047E-2</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>9.5300000000000003E-3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>8.6400000000000001E-3</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>9.8759999999999994E-3</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>9.9699999999999997E-3</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>8.1399999999999997E-3</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>8.9700000000000005E-3</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>9.7400000000000004E-3</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>1.137E-2</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <f t="shared" si="0"/>
         <v>9.637999999999999E-3</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>1.085E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>8.3599999999999994E-3</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>8.1600000000000006E-3</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>8.4739999999999989E-3</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1.358E-2</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>8.1700000000000002E-3</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>7.0499999999999998E-3</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>7.3200000000000001E-3</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>7.4900000000000001E-3</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>8.7219999999999989E-3</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -856,5 +1820,7 @@
     <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>